<commit_message>
Data file changed select rules column removed
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
+++ b/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
@@ -4,18 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7530"/>
+    <workbookView windowWidth="20490" windowHeight="7500"/>
   </bookViews>
   <sheets>
     <sheet name="SailPointApplicationJDBC" sheetId="2" r:id="rId1"/>
     <sheet name="DelimitedFile" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
   <si>
     <t>LOGIN DETAILS</t>
   </si>
@@ -27,9 +40,6 @@
   </si>
   <si>
     <t>CREATE RULES FOR APPLICATION IN RULES TAB</t>
-  </si>
-  <si>
-    <t>SELECTING RULE IN RULES TAB</t>
   </si>
   <si>
     <t>IDENTITY MAPPING OF APPLICATION</t>
@@ -225,14 +235,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,12 +309,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF1F1F1F"/>
-      <name val="Courier New"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF2A00FF"/>
       <name val="Courier New"/>
@@ -661,7 +665,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -692,32 +696,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -839,135 +817,135 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -995,18 +973,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1326,10 +1299,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="$A4:$XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1349,14 +1322,13 @@
     <col min="14" max="14" width="29.2857142857143" customWidth="1"/>
     <col min="15" max="15" width="28.5714285714286" customWidth="1"/>
     <col min="16" max="16" width="40" customWidth="1"/>
-    <col min="17" max="17" width="26.1428571428571" customWidth="1"/>
-    <col min="18" max="19" width="36.1428571428571" customWidth="1"/>
-    <col min="20" max="20" width="36.5714285714286" customWidth="1"/>
-    <col min="21" max="21" width="29.2857142857143" customWidth="1"/>
-    <col min="22" max="22" width="25.7142857142857" customWidth="1"/>
+    <col min="17" max="17" width="36.1428571428571" customWidth="1"/>
+    <col min="18" max="18" width="36.5714285714286" customWidth="1"/>
+    <col min="19" max="19" width="29.2857142857143" customWidth="1"/>
+    <col min="20" max="20" width="25.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" spans="1:22">
+    <row r="1" ht="23.25" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1384,161 +1356,144 @@
       <c r="Q1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="15" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="7" t="s">
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" ht="18.75" spans="1:20">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="7"/>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" ht="21" spans="1:22">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="V2" s="5" t="s">
+    <row r="3" ht="45" spans="1:20">
+      <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" ht="45" spans="1:22">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="N3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="Q3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="17" t="s">
-        <v>40</v>
+      <c r="R3" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="T3" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="V3" s="18" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1566,22 +1521,22 @@
   <sheetData>
     <row r="1" ht="18.75" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
Delimated XL File Added
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
+++ b/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="SailPointApplicationJDBC" sheetId="2" r:id="rId1"/>
-    <sheet name="DelimitedFile" sheetId="7" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>LOGIN DETAILS</t>
   </si>
@@ -222,18 +221,6 @@
   <si>
     <t>Delete</t>
   </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>DelimitedTxt</t>
-  </si>
-  <si>
-    <t>DelimitedIdentityAttribute</t>
-  </si>
-  <si>
-    <t>DelimitedDisplayAttribute</t>
-  </si>
 </sst>
 </file>
 
@@ -255,15 +242,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -471,19 +458,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -920,7 +907,7 @@
     <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -948,39 +935,38 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1303,13 +1289,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.5714285714286" customWidth="1"/>
@@ -1333,177 +1319,161 @@
   </cols>
   <sheetData>
     <row r="1" ht="23.25" spans="1:20">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="8" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="7"/>
+      <c r="N1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="14" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="9" t="s">
+      <c r="R1" s="13"/>
+      <c r="S1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="9"/>
+      <c r="T1" s="8"/>
     </row>
     <row r="2" ht="18.75" spans="1:20">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="S2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="15" t="s">
+      <c r="T2" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" ht="45" spans="1:20">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="N3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="O3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Q3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="R3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="S3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="15" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1518,57 +1488,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="26.7142857142857" customWidth="1"/>
-    <col min="2" max="2" width="27.1428571428571" customWidth="1"/>
-    <col min="3" max="3" width="24.5714285714286" customWidth="1"/>
-    <col min="4" max="4" width="26.5714285714286" customWidth="1"/>
-    <col min="5" max="5" width="34.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="40.5714285714286" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Up to Now Success....:)
</commit_message>
<xml_diff>
--- a/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
+++ b/src/test/resources/DataFiles/JDBCAPPLICATION.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>LOGIN DETAILS</t>
   </si>
@@ -47,6 +47,9 @@
     <t>DEBUG OPERATIONS</t>
   </si>
   <si>
+    <t>TASK ACTION</t>
+  </si>
+  <si>
     <t>username</t>
   </si>
   <si>
@@ -105,6 +108,9 @@
   </si>
   <si>
     <t>Action</t>
+  </si>
+  <si>
+    <t>TaskAction</t>
   </si>
   <si>
     <t>spadmin</t>
@@ -221,6 +227,54 @@
   <si>
     <t>Delete</t>
   </si>
+  <si>
+    <t>Execute In Background</t>
+  </si>
+  <si>
+    <t>EmployeeJDBC1</t>
+  </si>
+  <si>
+    <t>EmployeeJDBCAggregation</t>
+  </si>
+  <si>
+    <t>Create CorretionRulesail</t>
+  </si>
+  <si>
+    <t>DelimitedFile</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Account Group Aggregation</t>
+  </si>
+  <si>
+    <t>Creation Rule</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Manager Correlation Rule</t>
+  </si>
+  <si>
+    <t>Identity</t>
+  </si>
+  <si>
+    <t>Customization Rule</t>
+  </si>
+  <si>
+    <t>Managed Entitlement Customization Rule</t>
+  </si>
+  <si>
+    <t>Before Provisioning Rule</t>
+  </si>
+  <si>
+    <t>After Provisioning Rule</t>
+  </si>
 </sst>
 </file>
 
@@ -232,7 +286,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="30">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,6 +346,12 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -449,7 +509,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -476,6 +536,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -655,7 +727,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -686,6 +758,19 @@
         <color auto="1"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -807,74 +892,68 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -883,10 +962,10 @@
     <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -895,10 +974,10 @@
     <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -907,22 +986,22 @@
     <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -931,11 +1010,17 @@
     <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -951,6 +1036,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -963,13 +1050,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,13 +1385,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="13.5714285714286" customWidth="1"/>
@@ -1309,16 +1405,17 @@
     <col min="10" max="11" width="27.5714285714286" customWidth="1"/>
     <col min="12" max="12" width="29.2857142857143" customWidth="1"/>
     <col min="13" max="13" width="34.7142857142857" customWidth="1"/>
-    <col min="14" max="14" width="29.2857142857143" customWidth="1"/>
+    <col min="14" max="14" width="36" customWidth="1"/>
     <col min="15" max="15" width="28.5714285714286" customWidth="1"/>
     <col min="16" max="16" width="40" customWidth="1"/>
     <col min="17" max="17" width="36.1428571428571" customWidth="1"/>
     <col min="18" max="18" width="36.5714285714286" customWidth="1"/>
     <col min="19" max="19" width="29.2857142857143" customWidth="1"/>
     <col min="20" max="20" width="25.7142857142857" customWidth="1"/>
+    <col min="21" max="21" width="32.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="23.25" spans="1:20">
+    <row r="1" ht="23.25" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,146 +1431,356 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8" t="s">
+      <c r="M1" s="9"/>
+      <c r="N1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="13" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="13"/>
-      <c r="S1" s="8" t="s">
+      <c r="R1" s="19"/>
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="8"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="20" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" ht="18.75" spans="1:20">
+    <row r="2" ht="18.75" spans="1:21">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" ht="45" spans="1:21">
+      <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" ht="45" spans="1:21">
+      <c r="A4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="7">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>3</v>
+      </c>
+      <c r="E8" s="7">
+        <v>4</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="7">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="H8" s="7">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="I8" s="7">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="J8" s="7">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="K8" s="7">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="L8" s="7">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="M8" s="7">
         <v>12</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="N8" s="7">
         <v>13</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="O8" s="7">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="P8" s="7">
         <v>15</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="Q8" s="7">
         <v>16</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="R8" s="7">
         <v>17</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="S8" s="7">
         <v>18</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="T8" s="7">
         <v>19</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="U8" s="7">
         <v>20</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="T2" s="14" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="3" ht="45" spans="1:20">
-      <c r="A3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="6" t="s">
+    <row r="9" spans="5:21">
+      <c r="E9" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="5:21">
+      <c r="E10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>44</v>
+      <c r="M10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="14:21">
+      <c r="N11" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="14:14">
+      <c r="N12" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="14:14">
+      <c r="N13" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="14:14">
+      <c r="N14" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="14:14">
+      <c r="N15" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>